<commit_message>
creared FK_TypeOfPdo_PDO, models TypeOfPdo and JournalPDO, added tests
</commit_message>
<xml_diff>
--- a/docs/Таблицы для БД.xlsx
+++ b/docs/Таблицы для БД.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\KPandDP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AEFBE7-D0B2-43ED-93D6-BAB1FFC99D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64340111-2CF8-4D4A-B789-30508FE6D674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="248">
   <si>
     <t>Журнал ПОО</t>
   </si>
@@ -536,12 +536,6 @@
     <t>TypesOfElevators (Типы подъемников)</t>
   </si>
   <si>
-    <t>TypesOfLifts (Типы лифтов)</t>
-  </si>
-  <si>
-    <t>TypesOfLiftingCranes (Типы грузоподъемных кранов)</t>
-  </si>
-  <si>
     <t>Рафальский Д.Н.</t>
   </si>
   <si>
@@ -674,24 +668,15 @@
     <t>registrationNumber (регистрационный номер)</t>
   </si>
   <si>
-    <t>type (тип)</t>
-  </si>
-  <si>
     <t>dateOfRegistration (дата регистрации)</t>
   </si>
   <si>
     <t>technicalSpecifications (технические характеристики)</t>
   </si>
   <si>
-    <t>journalPDO (журнал ПОО)</t>
-  </si>
-  <si>
     <t>informationAboutTheTechnicalInspection (сведения о техническом освидетельствовании)</t>
   </si>
   <si>
-    <t>inspector (инспектор)</t>
-  </si>
-  <si>
     <t>TechnicalConditional (Техническое состояние)</t>
   </si>
   <si>
@@ -774,6 +759,18 @@
   </si>
   <si>
     <t>JournalPDOtoTS</t>
+  </si>
+  <si>
+    <t>journalPdoId (журнал ПОО)</t>
+  </si>
+  <si>
+    <t>typeId (тип)</t>
+  </si>
+  <si>
+    <t>inspectorId (инспектор)</t>
+  </si>
+  <si>
+    <t>TypeOfPDO (Тип ПОО)</t>
   </si>
 </sst>
 </file>
@@ -860,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -920,12 +917,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1001,27 +1007,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1031,12 +1047,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1046,6 +1056,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1058,19 +1071,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1080,6 +1080,23 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1418,34 +1435,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="E2" s="41" t="s">
+      <c r="C2" s="46"/>
+      <c r="E2" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="H2" s="37" t="s">
+      <c r="F2" s="47"/>
+      <c r="H2" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="K2" s="37" t="s">
+      <c r="I2" s="42"/>
+      <c r="K2" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="N2" s="37" t="s">
+      <c r="L2" s="42"/>
+      <c r="N2" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="Q2" s="37" t="s">
+      <c r="O2" s="42"/>
+      <c r="Q2" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="T2" s="37" t="s">
+      <c r="R2" s="42"/>
+      <c r="T2" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="U2" s="38"/>
+      <c r="U2" s="42"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
@@ -1658,10 +1675,10 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="42"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
         <v>96</v>
@@ -1734,36 +1751,36 @@
       <c r="F15" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="40"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="42" t="s">
+      <c r="K15" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="43"/>
+      <c r="L15" s="44"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="40" t="s">
+      <c r="N15" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="O15" s="40"/>
+      <c r="O15" s="45"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="40" t="s">
+      <c r="Q15" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="40"/>
+      <c r="R15" s="45"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="40" t="s">
+      <c r="T15" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="U15" s="40"/>
+      <c r="U15" s="45"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
@@ -1918,10 +1935,10 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="39"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="6"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12" t="s">
@@ -2284,10 +2301,10 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="38"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="6"/>
       <c r="F31" t="s">
         <v>97</v>
@@ -2511,10 +2528,10 @@
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="39"/>
+      <c r="C40" s="46"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
@@ -2535,10 +2552,10 @@
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="38"/>
+      <c r="C45" s="42"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
@@ -2559,10 +2576,10 @@
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="39"/>
+      <c r="C50" s="46"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
@@ -2614,12 +2631,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="B31:C31"/>
@@ -2633,6 +2644,12 @@
     <mergeCell ref="Q15:R15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="285" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2641,10 +2658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:AB60"/>
+  <dimension ref="B1:AD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2655,69 +2672,71 @@
     <col min="4" max="4" width="10.44140625" style="17" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="17"/>
     <col min="6" max="6" width="6.44140625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="42.5546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="49.5546875" style="17" customWidth="1"/>
     <col min="8" max="8" width="9" style="17" customWidth="1"/>
     <col min="9" max="9" width="8.88671875" style="17"/>
     <col min="10" max="10" width="30" style="17" customWidth="1"/>
-    <col min="11" max="11" width="10" style="17" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" style="17" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="15" style="17" customWidth="1"/>
-    <col min="16" max="17" width="8.88671875" style="17"/>
-    <col min="18" max="18" width="19.88671875" style="17" customWidth="1"/>
-    <col min="19" max="19" width="17.44140625" style="17" customWidth="1"/>
-    <col min="20" max="20" width="15.109375" style="17" customWidth="1"/>
-    <col min="21" max="21" width="29.44140625" style="17" customWidth="1"/>
-    <col min="22" max="23" width="8.88671875" style="17"/>
-    <col min="24" max="24" width="14.109375" style="17" customWidth="1"/>
-    <col min="25" max="26" width="8.88671875" style="17"/>
-    <col min="27" max="27" width="6.6640625" style="17" customWidth="1"/>
-    <col min="28" max="28" width="30.88671875" style="17" customWidth="1"/>
-    <col min="29" max="16384" width="8.88671875" style="17"/>
+    <col min="11" max="12" width="10" style="17" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" style="17" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" style="17" customWidth="1"/>
+    <col min="16" max="17" width="15" style="17" customWidth="1"/>
+    <col min="18" max="19" width="8.88671875" style="17"/>
+    <col min="20" max="20" width="19.88671875" style="17" customWidth="1"/>
+    <col min="21" max="21" width="17.44140625" style="17" customWidth="1"/>
+    <col min="22" max="22" width="15.109375" style="17" customWidth="1"/>
+    <col min="23" max="23" width="29.44140625" style="17" customWidth="1"/>
+    <col min="24" max="25" width="8.88671875" style="17"/>
+    <col min="26" max="26" width="14.109375" style="17" customWidth="1"/>
+    <col min="27" max="28" width="8.88671875" style="17"/>
+    <col min="29" max="29" width="6.6640625" style="17" customWidth="1"/>
+    <col min="30" max="30" width="30.88671875" style="17" customWidth="1"/>
+    <col min="31" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.3">
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="55"/>
-      <c r="F2" s="49" t="s">
+    <row r="2" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="57" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="F2" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="49"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="50" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="M2" s="53" t="s">
+      <c r="I2" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="64"/>
+      <c r="N2" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="Q2" s="51" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="62"/>
+      <c r="S2" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="52"/>
-      <c r="W2" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="63"/>
-      <c r="AA2" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="AB2" s="48"/>
-    </row>
-    <row r="3" spans="2:28" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="55"/>
+      <c r="Y2" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="61"/>
+      <c r="AC2" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD2" s="55"/>
+    </row>
+    <row r="3" spans="2:30" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
         <v>149</v>
       </c>
@@ -2737,355 +2756,370 @@
       <c r="J3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="L3" s="67"/>
+      <c r="N3" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="O3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="O3" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q3" s="19" t="s">
+      <c r="P3" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q3" s="63"/>
+      <c r="S3" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="R3" s="57" t="s">
+      <c r="T3" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="U3" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="V3" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="W3" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="S3" s="57" t="s">
-        <v>206</v>
-      </c>
-      <c r="T3" s="57" t="s">
-        <v>208</v>
-      </c>
-      <c r="U3" s="57" t="s">
-        <v>209</v>
-      </c>
-      <c r="W3" s="58" t="s">
+      <c r="Y3" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y3" s="58" t="s">
+      <c r="Z3" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA3" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="AA3" s="19" t="s">
+      <c r="AC3" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="AB3" s="20" t="s">
+      <c r="AD3" s="20" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="23">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="23">
         <v>1</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="M4" s="23">
+        <v>181</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>186</v>
+      </c>
+      <c r="L4" s="68"/>
+      <c r="N4" s="23">
         <v>1</v>
       </c>
-      <c r="N4" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="O4" s="23">
+      <c r="O4" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="P4" s="23">
         <v>31</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="27"/>
+      <c r="S4" s="23">
         <v>1</v>
       </c>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
       <c r="T4" s="23"/>
       <c r="U4" s="23"/>
-      <c r="W4" s="60">
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="Y4" s="40">
         <v>1</v>
       </c>
-      <c r="X4" s="60">
+      <c r="Z4" s="40">
         <v>31</v>
       </c>
-      <c r="Y4" s="60">
+      <c r="AA4" s="40">
         <v>1</v>
       </c>
-      <c r="AA4" s="23">
+      <c r="AC4" s="23">
         <v>1</v>
       </c>
-      <c r="AB4" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AD4" s="23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="23">
         <v>2</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F5" s="26">
         <v>2</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="23">
         <v>2</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="M5" s="23">
+        <v>182</v>
+      </c>
+      <c r="K5" s="66" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" s="68"/>
+      <c r="N5" s="23">
         <v>2</v>
       </c>
-      <c r="N5" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="O5" s="23">
+      <c r="O5" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="P5" s="23">
         <v>32</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="27"/>
+      <c r="S5" s="23">
         <v>2</v>
       </c>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
-      <c r="W5" s="60">
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="Y5" s="40">
         <v>2</v>
       </c>
-      <c r="X5" s="60">
+      <c r="Z5" s="40">
         <v>31</v>
       </c>
-      <c r="Y5" s="60">
+      <c r="AA5" s="40">
         <v>2</v>
       </c>
-      <c r="AA5" s="23">
+      <c r="AC5" s="23">
         <v>2</v>
       </c>
-      <c r="AB5" s="23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD5" s="23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23">
         <v>3</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F6" s="24">
         <v>3</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="23">
         <v>3</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="M6" s="23">
+        <v>238</v>
+      </c>
+      <c r="K6" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="L6" s="68"/>
+      <c r="N6" s="23">
         <v>3</v>
       </c>
-      <c r="N6" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="O6" s="23">
+      <c r="O6" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="P6" s="23">
         <v>33</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="27"/>
+      <c r="S6" s="23">
         <v>3</v>
       </c>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
-      <c r="W6" s="60">
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="Y6" s="40">
         <v>3</v>
       </c>
-      <c r="X6" s="60">
+      <c r="Z6" s="40">
         <v>32</v>
       </c>
-      <c r="Y6" s="60">
+      <c r="AA6" s="40">
         <v>1</v>
       </c>
-      <c r="AA6" s="23">
+      <c r="AC6" s="23">
         <v>3</v>
       </c>
-      <c r="AB6" s="23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AD6" s="23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B7" s="23">
         <v>4</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" s="24">
         <v>4</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="23">
         <v>4</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="M7" s="23">
+        <v>183</v>
+      </c>
+      <c r="K7" s="66" t="s">
+        <v>189</v>
+      </c>
+      <c r="L7" s="68"/>
+      <c r="N7" s="23">
         <v>4</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="O7" s="23">
+      <c r="O7" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="P7" s="23">
         <v>34</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="27"/>
+      <c r="S7" s="23">
         <v>4</v>
       </c>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
       <c r="T7" s="23"/>
       <c r="U7" s="23"/>
-      <c r="W7" s="60">
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="Y7" s="40">
         <v>4</v>
       </c>
-      <c r="X7" s="60">
+      <c r="Z7" s="40">
         <v>32</v>
       </c>
-      <c r="Y7" s="60">
+      <c r="AA7" s="40">
         <v>3</v>
       </c>
-      <c r="AA7" s="23">
+      <c r="AC7" s="23">
         <v>4</v>
       </c>
-      <c r="AB7" s="23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AD7" s="23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B8" s="23">
         <v>5</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F8" s="24">
         <v>5</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="23">
         <v>5</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="M8" s="23">
+        <v>184</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>190</v>
+      </c>
+      <c r="L8" s="68"/>
+      <c r="N8" s="23">
         <v>5</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="O8" s="23">
+      <c r="O8" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="P8" s="23">
         <v>36</v>
       </c>
-      <c r="W8" s="60">
+      <c r="Q8" s="27"/>
+      <c r="Y8" s="40">
         <v>5</v>
       </c>
-      <c r="X8" s="60">
+      <c r="Z8" s="40">
         <v>32</v>
       </c>
-      <c r="Y8" s="60">
+      <c r="AA8" s="40">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="F9" s="24">
         <v>6</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="23">
         <v>6</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B10" s="53" t="s">
-        <v>247</v>
-      </c>
-      <c r="C10" s="53"/>
+        <v>185</v>
+      </c>
+      <c r="K9" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="L9" s="68"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B10" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="56"/>
       <c r="F10" s="24">
         <v>7</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="23">
         <v>7</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="M10" s="27"/>
+        <v>192</v>
+      </c>
+      <c r="K10" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="L10" s="68"/>
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
-    </row>
-    <row r="11" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+    </row>
+    <row r="11" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>149</v>
       </c>
@@ -3097,65 +3131,76 @@
         <v>8</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="23">
         <v>8</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="M11" s="27"/>
+        <v>194</v>
+      </c>
+      <c r="K11" s="66" t="s">
+        <v>195</v>
+      </c>
+      <c r="L11" s="68"/>
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B12" s="29"/>
       <c r="C12" s="23" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D12" s="28"/>
       <c r="F12" s="24">
         <v>9</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="H12" s="18"/>
       <c r="I12" s="23">
         <v>9</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+      <c r="K12" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="L12" s="68"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B13" s="29"/>
       <c r="C13" s="23" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D13" s="27"/>
       <c r="F13" s="24">
         <v>10</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H13" s="18"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-    </row>
-    <row r="14" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I13" s="23">
+        <v>10</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="K13" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="L13" s="68"/>
+    </row>
+    <row r="14" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="29"/>
       <c r="C14" s="25" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
@@ -3163,16 +3208,24 @@
         <v>11</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H14" s="18"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="I14" s="23">
+        <v>11</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="L14" s="68"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -3180,33 +3233,46 @@
         <v>12</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H15" s="18"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
+      <c r="I15" s="23">
+        <v>12</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="L15" s="68"/>
+      <c r="M15" s="30"/>
+      <c r="R15" s="30"/>
       <c r="X15" s="30"/>
       <c r="Y15" s="30"/>
       <c r="Z15" s="30"/>
       <c r="AA15" s="30"/>
-      <c r="AB15" s="18"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB15" s="30"/>
+      <c r="AC15" s="30"/>
+      <c r="AD15" s="18"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="23"/>
       <c r="C16" s="23" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D16" s="27"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
+      <c r="I16" s="23">
+        <v>13</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="68"/>
       <c r="M16" s="30"/>
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
@@ -3222,17 +3288,23 @@
       <c r="Y16" s="30"/>
       <c r="Z16" s="30"/>
       <c r="AA16" s="30"/>
-      <c r="AB16" s="18"/>
-    </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="30"/>
+      <c r="AD16" s="18"/>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="E17" s="28"/>
       <c r="H17" s="18"/>
-      <c r="I17" s="53" t="s">
-        <v>169</v>
-      </c>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="30"/>
+      <c r="I17" s="23">
+        <v>14</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="68"/>
       <c r="M17" s="30"/>
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
@@ -3248,26 +3320,28 @@
       <c r="Y17" s="30"/>
       <c r="Z17" s="30"/>
       <c r="AA17" s="30"/>
-      <c r="AB17" s="18"/>
-    </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B18" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="46"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="18"/>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B18" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="58"/>
       <c r="D18" s="28"/>
       <c r="E18" s="27"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="L18" s="30"/>
+      <c r="I18" s="23">
+        <v>15</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="68"/>
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
@@ -3283,9 +3357,11 @@
       <c r="Y18" s="30"/>
       <c r="Z18" s="30"/>
       <c r="AA18" s="30"/>
-      <c r="AB18" s="18"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="30"/>
+      <c r="AD18" s="18"/>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>149</v>
       </c>
@@ -3294,15 +3370,9 @@
       </c>
       <c r="D19" s="27"/>
       <c r="H19" s="18"/>
-      <c r="I19" s="23">
-        <v>1</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="K19" s="23" t="s">
-        <v>201</v>
-      </c>
+      <c r="I19" s="27"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
       <c r="N19" s="30"/>
@@ -3319,31 +3389,27 @@
       <c r="Y19" s="30"/>
       <c r="Z19" s="30"/>
       <c r="AA19" s="30"/>
-      <c r="AB19" s="18"/>
-    </row>
-    <row r="20" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB19" s="30"/>
+      <c r="AC19" s="30"/>
+      <c r="AD19" s="18"/>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B20" s="23">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="28"/>
       <c r="H20" s="18"/>
-      <c r="I20" s="23">
-        <v>2</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>203</v>
-      </c>
+      <c r="I20" s="27"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="23"/>
       <c r="P20" s="30"/>
       <c r="Q20" s="30"/>
       <c r="R20" s="30"/>
@@ -3356,26 +3422,22 @@
       <c r="Y20" s="30"/>
       <c r="Z20" s="30"/>
       <c r="AA20" s="30"/>
-      <c r="AB20" s="18"/>
-    </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB20" s="30"/>
+      <c r="AC20" s="30"/>
+      <c r="AD20" s="18"/>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="23">
         <v>2</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E21" s="27"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="23">
-        <v>3</v>
-      </c>
-      <c r="J21" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="K21" s="23" t="s">
-        <v>205</v>
-      </c>
+      <c r="I21" s="27"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
       <c r="L21" s="30"/>
       <c r="M21" s="30"/>
       <c r="N21" s="30"/>
@@ -3392,27 +3454,25 @@
       <c r="Y21" s="30"/>
       <c r="Z21" s="30"/>
       <c r="AA21" s="30"/>
-      <c r="AB21" s="18"/>
-    </row>
-    <row r="22" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB21" s="30"/>
+      <c r="AC21" s="30"/>
+      <c r="AD21" s="18"/>
+    </row>
+    <row r="22" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="23">
         <v>3</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="27"/>
-      <c r="I22" s="23">
-        <v>4</v>
-      </c>
-      <c r="J22" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="L22" s="30"/>
+      <c r="I22" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="30"/>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
@@ -3428,27 +3488,29 @@
       <c r="Y22" s="30"/>
       <c r="Z22" s="30"/>
       <c r="AA22" s="30"/>
-      <c r="AB22" s="18"/>
-    </row>
-    <row r="23" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB22" s="30"/>
+      <c r="AC22" s="30"/>
+      <c r="AD22" s="18"/>
+    </row>
+    <row r="23" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="23">
         <v>4</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
-      <c r="I23" s="23">
-        <v>5</v>
-      </c>
-      <c r="J23" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L23" s="30"/>
+      <c r="I23" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="L23" s="63"/>
       <c r="M23" s="30"/>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
@@ -3464,14 +3526,16 @@
       <c r="Y23" s="30"/>
       <c r="Z23" s="30"/>
       <c r="AA23" s="30"/>
-      <c r="AB23" s="18"/>
-    </row>
-    <row r="24" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB23" s="30"/>
+      <c r="AC23" s="30"/>
+      <c r="AD23" s="18"/>
+    </row>
+    <row r="24" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="23">
         <v>5</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
@@ -3479,15 +3543,15 @@
         <v>97</v>
       </c>
       <c r="I24" s="23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>35</v>
+        <v>153</v>
       </c>
       <c r="K24" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="L24" s="30"/>
+        <v>154</v>
+      </c>
+      <c r="L24" s="27"/>
       <c r="M24" s="30"/>
       <c r="N24" s="30"/>
       <c r="O24" s="30"/>
@@ -3503,21 +3567,29 @@
       <c r="Y24" s="30"/>
       <c r="Z24" s="30"/>
       <c r="AA24" s="30"/>
-      <c r="AB24" s="18"/>
-    </row>
-    <row r="25" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB24" s="30"/>
+      <c r="AC24" s="30"/>
+      <c r="AD24" s="18"/>
+    </row>
+    <row r="25" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="23">
         <v>6</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
+      <c r="I25" s="23">
+        <v>2</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="27"/>
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
       <c r="O25" s="30"/>
@@ -3533,14 +3605,16 @@
       <c r="Y25" s="30"/>
       <c r="Z25" s="30"/>
       <c r="AA25" s="30"/>
-      <c r="AB25" s="18"/>
-    </row>
-    <row r="26" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB25" s="30"/>
+      <c r="AC25" s="30"/>
+      <c r="AD25" s="18"/>
+    </row>
+    <row r="26" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="23">
         <v>7</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
@@ -3563,9 +3637,11 @@
       <c r="Y26" s="30"/>
       <c r="Z26" s="30"/>
       <c r="AA26" s="30"/>
-      <c r="AB26" s="18"/>
-    </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB26" s="30"/>
+      <c r="AC26" s="30"/>
+      <c r="AD26" s="18"/>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="D27" s="27"/>
       <c r="E27" s="31"/>
       <c r="I27" s="27"/>
@@ -3587,21 +3663,23 @@
       <c r="Y27" s="30"/>
       <c r="Z27" s="30"/>
       <c r="AA27" s="30"/>
-      <c r="AB27" s="18"/>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B28" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C28" s="44"/>
+      <c r="AB27" s="30"/>
+      <c r="AC27" s="30"/>
+      <c r="AD27" s="18"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B28" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="48"/>
       <c r="D28" s="27"/>
       <c r="E28" s="31"/>
-      <c r="I28" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="30"/>
+      <c r="I28" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="28"/>
       <c r="M28" s="30"/>
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
@@ -3617,9 +3695,11 @@
       <c r="Y28" s="30"/>
       <c r="Z28" s="30"/>
       <c r="AA28" s="30"/>
-      <c r="AB28" s="18"/>
-    </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB28" s="30"/>
+      <c r="AC28" s="30"/>
+      <c r="AD28" s="18"/>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="19" t="s">
         <v>149</v>
       </c>
@@ -3636,7 +3716,7 @@
       <c r="K29" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L29" s="30"/>
+      <c r="L29" s="63"/>
       <c r="M29" s="30"/>
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
@@ -3652,12 +3732,14 @@
       <c r="Y29" s="30"/>
       <c r="Z29" s="30"/>
       <c r="AA29" s="30"/>
-      <c r="AB29" s="18"/>
-    </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB29" s="30"/>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="18"/>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" s="29"/>
       <c r="C30" s="23" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="28"/>
@@ -3665,12 +3747,12 @@
         <v>1</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="K30" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="L30" s="30"/>
+        <v>157</v>
+      </c>
+      <c r="L30" s="27"/>
       <c r="M30" s="30"/>
       <c r="N30" s="30"/>
       <c r="O30" s="30"/>
@@ -3686,12 +3768,14 @@
       <c r="Y30" s="30"/>
       <c r="Z30" s="30"/>
       <c r="AA30" s="30"/>
-      <c r="AB30" s="18"/>
-    </row>
-    <row r="31" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB30" s="30"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="18"/>
+    </row>
+    <row r="31" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="23"/>
       <c r="C31" s="25" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="27"/>
@@ -3699,12 +3783,12 @@
         <v>2</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K31" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" s="30"/>
+        <v>158</v>
+      </c>
+      <c r="L31" s="27"/>
       <c r="M31" s="30"/>
       <c r="N31" s="30"/>
       <c r="O31" s="30"/>
@@ -3720,16 +3804,16 @@
       <c r="Y31" s="30"/>
       <c r="Z31" s="30"/>
       <c r="AA31" s="30"/>
-      <c r="AB31" s="18"/>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB31" s="30"/>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="18"/>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B32" s="23"/>
       <c r="C32" s="23" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="30"/>
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
@@ -3747,13 +3831,13 @@
       <c r="Y32" s="30"/>
       <c r="Z32" s="30"/>
       <c r="AA32" s="30"/>
-      <c r="AB32" s="18"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB32" s="30"/>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="18"/>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
       <c r="D33" s="28"/>
       <c r="E33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="30"/>
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
@@ -3771,21 +3855,23 @@
       <c r="Y33" s="30"/>
       <c r="Z33" s="30"/>
       <c r="AA33" s="30"/>
-      <c r="AB33" s="18"/>
-    </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B34" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34" s="46"/>
+      <c r="AB33" s="30"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="18"/>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B34" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="50"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
-      <c r="I34" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="30"/>
+      <c r="I34" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="28"/>
       <c r="M34" s="30"/>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
@@ -3801,9 +3887,11 @@
       <c r="Y34" s="30"/>
       <c r="Z34" s="30"/>
       <c r="AA34" s="30"/>
-      <c r="AB34" s="18"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB34" s="30"/>
+      <c r="AC34" s="30"/>
+      <c r="AD34" s="18"/>
+    </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B35" s="19" t="s">
         <v>149</v>
       </c>
@@ -3821,7 +3909,7 @@
       <c r="K35" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L35" s="30"/>
+      <c r="L35" s="63"/>
       <c r="M35" s="30"/>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -3837,24 +3925,26 @@
       <c r="Y35" s="30"/>
       <c r="Z35" s="30"/>
       <c r="AA35" s="30"/>
-      <c r="AB35" s="18"/>
-    </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB35" s="30"/>
+      <c r="AC35" s="30"/>
+      <c r="AD35" s="18"/>
+    </row>
+    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B36" s="32"/>
       <c r="C36" s="23" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D36" s="27"/>
       <c r="I36" s="23">
         <v>1</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="L36" s="30"/>
+        <v>160</v>
+      </c>
+      <c r="L36" s="27"/>
       <c r="M36" s="30"/>
       <c r="N36" s="30"/>
       <c r="O36" s="30"/>
@@ -3870,24 +3960,26 @@
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
       <c r="AA36" s="30"/>
-      <c r="AB36" s="18"/>
-    </row>
-    <row r="37" spans="2:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AB36" s="30"/>
+      <c r="AC36" s="30"/>
+      <c r="AD36" s="18"/>
+    </row>
+    <row r="37" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B37" s="23"/>
       <c r="C37" s="25" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D37" s="27"/>
       <c r="I37" s="23">
         <v>2</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="K37" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="L37" s="30"/>
+        <v>162</v>
+      </c>
+      <c r="L37" s="27"/>
       <c r="M37" s="30"/>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -3903,16 +3995,26 @@
       <c r="Y37" s="30"/>
       <c r="Z37" s="30"/>
       <c r="AA37" s="30"/>
-      <c r="AB37" s="18"/>
-    </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB37" s="30"/>
+      <c r="AC37" s="30"/>
+      <c r="AD37" s="18"/>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B38" s="23"/>
       <c r="C38" s="23" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D38" s="27"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
+      <c r="I38" s="23">
+        <v>2</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="L38" s="27"/>
       <c r="M38" s="30"/>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
@@ -3928,12 +4030,12 @@
       <c r="Y38" s="30"/>
       <c r="Z38" s="30"/>
       <c r="AA38" s="30"/>
-      <c r="AB38" s="18"/>
-    </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB38" s="30"/>
+      <c r="AC38" s="30"/>
+      <c r="AD38" s="18"/>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
       <c r="D39" s="27"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
       <c r="M39" s="30"/>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -3949,20 +4051,16 @@
       <c r="Y39" s="30"/>
       <c r="Z39" s="30"/>
       <c r="AA39" s="30"/>
-      <c r="AB39" s="18"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B40" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="C40" s="44"/>
+      <c r="AB39" s="30"/>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="18"/>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B40" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="48"/>
       <c r="D40" s="31"/>
-      <c r="I40" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="30"/>
       <c r="M40" s="30"/>
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
@@ -3978,29 +4076,23 @@
       <c r="Y40" s="30"/>
       <c r="Z40" s="30"/>
       <c r="AA40" s="30"/>
-      <c r="AB40" s="18"/>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="18"/>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B41" s="19" t="s">
         <v>149</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="I41" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="J41" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="K41" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="M41" s="30"/>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
-    </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B42" s="23">
         <v>1</v>
       </c>
@@ -4009,17 +4101,8 @@
       </c>
       <c r="D42" s="28"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="23">
-        <v>1</v>
-      </c>
-      <c r="J42" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="K42" s="23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B43" s="23">
         <v>2</v>
       </c>
@@ -4028,17 +4111,8 @@
       </c>
       <c r="D43" s="27"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="23">
-        <v>2</v>
-      </c>
-      <c r="J43" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K43" s="23" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B44" s="23">
         <v>3</v>
       </c>
@@ -4047,17 +4121,8 @@
       </c>
       <c r="D44" s="27"/>
       <c r="H44" s="27"/>
-      <c r="I44" s="23">
-        <v>2</v>
-      </c>
-      <c r="J44" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="K44" s="23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B45" s="23">
         <v>4</v>
       </c>
@@ -4067,7 +4132,7 @@
       <c r="D45" s="27"/>
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B46" s="23">
         <v>5</v>
       </c>
@@ -4076,7 +4141,7 @@
       </c>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B47" s="23">
         <v>6</v>
       </c>
@@ -4086,7 +4151,7 @@
       <c r="D47" s="28"/>
       <c r="H47" s="27"/>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B48" s="23">
         <v>7</v>
       </c>
@@ -4135,23 +4200,22 @@
       <c r="D60" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I34:K34"/>
     <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I17:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="285" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactoring BD and test's code
</commit_message>
<xml_diff>
--- a/docs/Таблицы для БД.xlsx
+++ b/docs/Таблицы для БД.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\KPandDP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64340111-2CF8-4D4A-B789-30508FE6D674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43964C26-D433-440A-BBA6-CBEFBB038150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="253">
   <si>
     <t>Журнал ПОО</t>
   </si>
@@ -485,9 +485,6 @@
     <t>PDO (Потенциально опасный объект)</t>
   </si>
   <si>
-    <t>KeyTS</t>
-  </si>
-  <si>
     <t>эскалатор поэтажный</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
     <t>Смоловик Г.В.</t>
   </si>
   <si>
-    <t>Ведомственная принадлежность</t>
-  </si>
-  <si>
     <t>InstallationLocation (Место установки)</t>
   </si>
   <si>
@@ -758,9 +752,6 @@
     <t>Subjects (Субъект промышленной безопасности)</t>
   </si>
   <si>
-    <t>JournalPDOtoTS</t>
-  </si>
-  <si>
     <t>journalPdoId (журнал ПОО)</t>
   </si>
   <si>
@@ -771,6 +762,30 @@
   </si>
   <si>
     <t>TypeOfPDO (Тип ПОО)</t>
+  </si>
+  <si>
+    <t>GomelRegionalExecutiveCommittee (Гомельский облисполком)</t>
+  </si>
+  <si>
+    <t>MinistryOfIndustry (Министерство промышленности)</t>
+  </si>
+  <si>
+    <t>MinistryOfHealth (Министерство здравоохранения)</t>
+  </si>
+  <si>
+    <t>MinistryOfEnergy (Министерство энергетики)</t>
+  </si>
+  <si>
+    <t>MinistryOfEducation (Министерство образования)</t>
+  </si>
+  <si>
+    <t>Belneftekhim (Белнефтехим)</t>
+  </si>
+  <si>
+    <t>Bellesbumprom (Беллесбумпром)</t>
+  </si>
+  <si>
+    <t>DepartmentalAffiliation (Ведомственная принадлежность)</t>
   </si>
 </sst>
 </file>
@@ -831,7 +846,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,12 +862,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,7 +940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1010,76 +1019,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1097,6 +1036,60 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1435,34 +1428,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="E2" s="47" t="s">
+      <c r="C2" s="49"/>
+      <c r="E2" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="H2" s="41" t="s">
+      <c r="F2" s="48"/>
+      <c r="H2" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="K2" s="41" t="s">
+      <c r="I2" s="46"/>
+      <c r="K2" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="N2" s="41" t="s">
+      <c r="L2" s="46"/>
+      <c r="N2" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="Q2" s="41" t="s">
+      <c r="O2" s="46"/>
+      <c r="Q2" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="T2" s="41" t="s">
+      <c r="R2" s="46"/>
+      <c r="T2" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="U2" s="42"/>
+      <c r="U2" s="46"/>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
@@ -1675,10 +1668,10 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="46"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
         <v>96</v>
@@ -1751,36 +1744,36 @@
       <c r="F15" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="45"/>
+      <c r="I15" s="47"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="43" t="s">
+      <c r="K15" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="44"/>
+      <c r="L15" s="51"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="45" t="s">
+      <c r="N15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="O15" s="45"/>
+      <c r="O15" s="47"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="45" t="s">
+      <c r="Q15" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="45"/>
+      <c r="R15" s="47"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="45" t="s">
+      <c r="T15" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="U15" s="45"/>
+      <c r="U15" s="47"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12" t="s">
@@ -1935,10 +1928,10 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="46"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="6"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12" t="s">
@@ -2301,10 +2294,10 @@
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="42"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="6"/>
       <c r="F31" t="s">
         <v>97</v>
@@ -2528,10 +2521,10 @@
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="46"/>
+      <c r="C40" s="49"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
@@ -2552,10 +2545,10 @@
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C45" s="42"/>
+      <c r="C45" s="46"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B46" s="5"/>
@@ -2576,10 +2569,10 @@
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="46"/>
+      <c r="C50" s="49"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
@@ -2631,6 +2624,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="B31:C31"/>
@@ -2647,9 +2643,6 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="285" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2658,10 +2651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:AD60"/>
+  <dimension ref="B1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2687,56 +2680,49 @@
     <col min="22" max="22" width="15.109375" style="17" customWidth="1"/>
     <col min="23" max="23" width="29.44140625" style="17" customWidth="1"/>
     <col min="24" max="25" width="8.88671875" style="17"/>
-    <col min="26" max="26" width="14.109375" style="17" customWidth="1"/>
-    <col min="27" max="28" width="8.88671875" style="17"/>
-    <col min="29" max="29" width="6.6640625" style="17" customWidth="1"/>
-    <col min="30" max="30" width="30.88671875" style="17" customWidth="1"/>
-    <col min="31" max="16384" width="8.88671875" style="17"/>
+    <col min="26" max="26" width="6.6640625" style="17" customWidth="1"/>
+    <col min="27" max="27" width="30.88671875" style="17" customWidth="1"/>
+    <col min="28" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.3">
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="58"/>
-      <c r="F2" s="51" t="s">
+    <row r="2" spans="2:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="61" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="62"/>
+      <c r="F2" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="51"/>
+      <c r="G2" s="57"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="52" t="s">
-        <v>247</v>
-      </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="64"/>
-      <c r="N2" s="56" t="s">
+      <c r="I2" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="40"/>
+      <c r="N2" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="62"/>
-      <c r="S2" s="53" t="s">
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="38"/>
+      <c r="S2" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="55"/>
-      <c r="Y2" s="59" t="s">
-        <v>243</v>
-      </c>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="61"/>
-      <c r="AC2" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="AD2" s="55"/>
-    </row>
-    <row r="3" spans="2:30" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="56"/>
+      <c r="Z2" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA2" s="56"/>
+    </row>
+    <row r="3" spans="2:27" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
         <v>149</v>
       </c>
@@ -2756,10 +2742,10 @@
       <c r="J3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="L3" s="67"/>
+      <c r="L3" s="43"/>
       <c r="N3" s="19" t="s">
         <v>149</v>
       </c>
@@ -2767,69 +2753,60 @@
         <v>146</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q3" s="63"/>
+        <v>173</v>
+      </c>
+      <c r="Q3" s="39"/>
       <c r="S3" s="19" t="s">
         <v>149</v>
       </c>
       <c r="T3" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="U3" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="V3" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="W3" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="U3" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="V3" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="W3" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y3" s="38" t="s">
+      <c r="Z3" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="Z3" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="AA3" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="AC3" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD3" s="20" t="s">
+      <c r="AA3" s="20" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" s="23">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="23">
         <v>1</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="K4" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="L4" s="68"/>
+        <v>179</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="L4" s="44"/>
       <c r="N4" s="23">
         <v>1</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P4" s="23">
         <v>31</v>
@@ -2842,51 +2819,42 @@
       <c r="U4" s="23"/>
       <c r="V4" s="23"/>
       <c r="W4" s="23"/>
-      <c r="Y4" s="40">
+      <c r="Z4" s="23">
         <v>1</v>
       </c>
-      <c r="Z4" s="40">
-        <v>31</v>
-      </c>
-      <c r="AA4" s="40">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="23">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="23" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA4" s="23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B5" s="23">
         <v>2</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F5" s="26">
         <v>2</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="23">
         <v>2</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="K5" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="L5" s="68"/>
+        <v>180</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="L5" s="44"/>
       <c r="N5" s="23">
         <v>2</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P5" s="23">
         <v>32</v>
@@ -2899,51 +2867,42 @@
       <c r="U5" s="23"/>
       <c r="V5" s="23"/>
       <c r="W5" s="23"/>
-      <c r="Y5" s="40">
+      <c r="Z5" s="23">
         <v>2</v>
       </c>
-      <c r="Z5" s="40">
-        <v>31</v>
-      </c>
-      <c r="AA5" s="40">
-        <v>2</v>
-      </c>
-      <c r="AC5" s="23">
-        <v>2</v>
-      </c>
-      <c r="AD5" s="23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA5" s="23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23">
         <v>3</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F6" s="24">
         <v>3</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="23">
         <v>3</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="K6" s="66" t="s">
-        <v>188</v>
-      </c>
-      <c r="L6" s="68"/>
+        <v>236</v>
+      </c>
+      <c r="K6" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" s="44"/>
       <c r="N6" s="23">
         <v>3</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P6" s="23">
         <v>33</v>
@@ -2956,51 +2915,42 @@
       <c r="U6" s="23"/>
       <c r="V6" s="23"/>
       <c r="W6" s="23"/>
-      <c r="Y6" s="40">
+      <c r="Z6" s="23">
         <v>3</v>
       </c>
-      <c r="Z6" s="40">
-        <v>32</v>
-      </c>
-      <c r="AA6" s="40">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="23">
-        <v>3</v>
-      </c>
-      <c r="AD6" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA6" s="23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B7" s="23">
         <v>4</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7" s="24">
         <v>4</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="23">
         <v>4</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="K7" s="66" t="s">
-        <v>189</v>
-      </c>
-      <c r="L7" s="68"/>
+        <v>181</v>
+      </c>
+      <c r="K7" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="44"/>
       <c r="N7" s="23">
         <v>4</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P7" s="23">
         <v>34</v>
@@ -3013,113 +2963,95 @@
       <c r="U7" s="23"/>
       <c r="V7" s="23"/>
       <c r="W7" s="23"/>
-      <c r="Y7" s="40">
+      <c r="Z7" s="23">
         <v>4</v>
       </c>
-      <c r="Z7" s="40">
-        <v>32</v>
-      </c>
-      <c r="AA7" s="40">
-        <v>3</v>
-      </c>
-      <c r="AC7" s="23">
-        <v>4</v>
-      </c>
-      <c r="AD7" s="23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA7" s="23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B8" s="23">
         <v>5</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F8" s="24">
         <v>5</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="23">
         <v>5</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="K8" s="66" t="s">
-        <v>190</v>
-      </c>
-      <c r="L8" s="68"/>
+        <v>182</v>
+      </c>
+      <c r="K8" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="L8" s="44"/>
       <c r="N8" s="23">
         <v>5</v>
       </c>
       <c r="O8" s="23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="P8" s="23">
         <v>36</v>
       </c>
       <c r="Q8" s="27"/>
-      <c r="Y8" s="40">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="40">
-        <v>32</v>
-      </c>
-      <c r="AA8" s="40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="F9" s="24">
         <v>6</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="23">
         <v>6</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="K9" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="L9" s="68"/>
-    </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B10" s="56" t="s">
-        <v>242</v>
-      </c>
-      <c r="C10" s="56"/>
+        <v>183</v>
+      </c>
+      <c r="K9" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="L9" s="44"/>
+    </row>
+    <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="58"/>
       <c r="F10" s="24">
         <v>7</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="23">
         <v>7</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="L10" s="68"/>
+        <v>190</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="L10" s="44"/>
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
     </row>
-    <row r="11" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>149</v>
       </c>
@@ -3131,76 +3063,76 @@
         <v>8</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="23">
         <v>8</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="K11" s="66" t="s">
-        <v>195</v>
-      </c>
-      <c r="L11" s="68"/>
+        <v>192</v>
+      </c>
+      <c r="K11" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="L11" s="44"/>
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B12" s="29"/>
       <c r="C12" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D12" s="28"/>
       <c r="F12" s="24">
         <v>9</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H12" s="18"/>
       <c r="I12" s="23">
         <v>9</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="K12" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="L12" s="68"/>
-    </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+      <c r="K12" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="L12" s="44"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="29"/>
       <c r="C13" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D13" s="27"/>
       <c r="F13" s="24">
         <v>10</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="23">
         <v>10</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="K13" s="66" t="s">
-        <v>199</v>
-      </c>
-      <c r="L13" s="68"/>
-    </row>
-    <row r="14" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+      <c r="K13" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="L13" s="44"/>
+    </row>
+    <row r="14" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="29"/>
       <c r="C14" s="25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
@@ -3208,24 +3140,24 @@
         <v>11</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="23">
         <v>11</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="K14" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="L14" s="68"/>
-    </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="K14" s="42" t="s">
+        <v>199</v>
+      </c>
+      <c r="L14" s="44"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
@@ -3233,33 +3165,30 @@
         <v>12</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="23">
         <v>12</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="K15" s="66" t="s">
-        <v>203</v>
-      </c>
-      <c r="L15" s="68"/>
+        <v>200</v>
+      </c>
+      <c r="K15" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="L15" s="44"/>
       <c r="M15" s="30"/>
       <c r="R15" s="30"/>
       <c r="X15" s="30"/>
       <c r="Y15" s="30"/>
       <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
-      <c r="AB15" s="30"/>
-      <c r="AC15" s="30"/>
-      <c r="AD15" s="18"/>
-    </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA15" s="18"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B16" s="23"/>
       <c r="C16" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D16" s="27"/>
       <c r="H16" s="18"/>
@@ -3269,10 +3198,10 @@
       <c r="J16" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="66" t="s">
+      <c r="K16" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="68"/>
+      <c r="L16" s="44"/>
       <c r="M16" s="30"/>
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
@@ -3287,12 +3216,9 @@
       <c r="X16" s="30"/>
       <c r="Y16" s="30"/>
       <c r="Z16" s="30"/>
-      <c r="AA16" s="30"/>
-      <c r="AB16" s="30"/>
-      <c r="AC16" s="30"/>
-      <c r="AD16" s="18"/>
-    </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA16" s="18"/>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
       <c r="E17" s="28"/>
       <c r="H17" s="18"/>
       <c r="I17" s="23">
@@ -3301,10 +3227,10 @@
       <c r="J17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="68"/>
+      <c r="L17" s="44"/>
       <c r="M17" s="30"/>
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
@@ -3319,16 +3245,13 @@
       <c r="X17" s="30"/>
       <c r="Y17" s="30"/>
       <c r="Z17" s="30"/>
-      <c r="AA17" s="30"/>
-      <c r="AB17" s="30"/>
-      <c r="AC17" s="30"/>
-      <c r="AD17" s="18"/>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B18" s="57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="58"/>
+      <c r="AA17" s="18"/>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B18" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="62"/>
       <c r="D18" s="28"/>
       <c r="E18" s="27"/>
       <c r="H18" s="18"/>
@@ -3338,10 +3261,10 @@
       <c r="J18" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="66" t="s">
+      <c r="K18" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="L18" s="68"/>
+      <c r="L18" s="44"/>
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
@@ -3356,12 +3279,9 @@
       <c r="X18" s="30"/>
       <c r="Y18" s="30"/>
       <c r="Z18" s="30"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="30"/>
-      <c r="AC18" s="30"/>
-      <c r="AD18" s="18"/>
-    </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA18" s="18"/>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>149</v>
       </c>
@@ -3388,17 +3308,14 @@
       <c r="X19" s="30"/>
       <c r="Y19" s="30"/>
       <c r="Z19" s="30"/>
-      <c r="AA19" s="30"/>
-      <c r="AB19" s="30"/>
-      <c r="AC19" s="30"/>
-      <c r="AD19" s="18"/>
-    </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA19" s="18"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" s="23">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="28"/>
@@ -3421,17 +3338,14 @@
       <c r="X20" s="30"/>
       <c r="Y20" s="30"/>
       <c r="Z20" s="30"/>
-      <c r="AA20" s="30"/>
-      <c r="AB20" s="30"/>
-      <c r="AC20" s="30"/>
-      <c r="AD20" s="18"/>
-    </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA20" s="18"/>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="23">
         <v>2</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E21" s="27"/>
       <c r="H21" s="18"/>
@@ -3453,25 +3367,22 @@
       <c r="X21" s="30"/>
       <c r="Y21" s="30"/>
       <c r="Z21" s="30"/>
-      <c r="AA21" s="30"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="30"/>
-      <c r="AD21" s="18"/>
-    </row>
-    <row r="22" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA21" s="18"/>
+    </row>
+    <row r="22" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="23">
         <v>3</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="27"/>
-      <c r="I22" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
+      <c r="I22" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="28"/>
       <c r="M22" s="30"/>
       <c r="N22" s="30"/>
@@ -3487,17 +3398,14 @@
       <c r="X22" s="30"/>
       <c r="Y22" s="30"/>
       <c r="Z22" s="30"/>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30"/>
-      <c r="AC22" s="30"/>
-      <c r="AD22" s="18"/>
-    </row>
-    <row r="23" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA22" s="18"/>
+    </row>
+    <row r="23" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="23">
         <v>4</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -3510,7 +3418,7 @@
       <c r="K23" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L23" s="63"/>
+      <c r="L23" s="39"/>
       <c r="M23" s="30"/>
       <c r="N23" s="30"/>
       <c r="O23" s="30"/>
@@ -3525,17 +3433,14 @@
       <c r="X23" s="30"/>
       <c r="Y23" s="30"/>
       <c r="Z23" s="30"/>
-      <c r="AA23" s="30"/>
-      <c r="AB23" s="30"/>
-      <c r="AC23" s="30"/>
-      <c r="AD23" s="18"/>
-    </row>
-    <row r="24" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA23" s="18"/>
+    </row>
+    <row r="24" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="23">
         <v>5</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
@@ -3546,10 +3451,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>153</v>
-      </c>
-      <c r="K24" s="23" t="s">
-        <v>154</v>
       </c>
       <c r="L24" s="27"/>
       <c r="M24" s="30"/>
@@ -3566,17 +3471,14 @@
       <c r="X24" s="30"/>
       <c r="Y24" s="30"/>
       <c r="Z24" s="30"/>
-      <c r="AA24" s="30"/>
-      <c r="AB24" s="30"/>
-      <c r="AC24" s="30"/>
-      <c r="AD24" s="18"/>
-    </row>
-    <row r="25" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA24" s="18"/>
+    </row>
+    <row r="25" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="23">
         <v>6</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -3584,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K25" s="23" t="s">
         <v>14</v>
@@ -3604,17 +3506,14 @@
       <c r="X25" s="30"/>
       <c r="Y25" s="30"/>
       <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="18"/>
-    </row>
-    <row r="26" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA25" s="18"/>
+    </row>
+    <row r="26" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="23">
         <v>7</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
@@ -3636,12 +3535,9 @@
       <c r="X26" s="30"/>
       <c r="Y26" s="30"/>
       <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="18"/>
-    </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA26" s="18"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D27" s="27"/>
       <c r="E27" s="31"/>
       <c r="I27" s="27"/>
@@ -3662,23 +3558,20 @@
       <c r="X27" s="30"/>
       <c r="Y27" s="30"/>
       <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="18"/>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B28" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="48"/>
+      <c r="AA27" s="18"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B28" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" s="58"/>
       <c r="D28" s="27"/>
       <c r="E28" s="31"/>
-      <c r="I28" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
+      <c r="I28" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
       <c r="L28" s="28"/>
       <c r="M28" s="30"/>
       <c r="N28" s="30"/>
@@ -3694,12 +3587,9 @@
       <c r="X28" s="30"/>
       <c r="Y28" s="30"/>
       <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="30"/>
-      <c r="AC28" s="30"/>
-      <c r="AD28" s="18"/>
-    </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA28" s="18"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B29" s="19" t="s">
         <v>149</v>
       </c>
@@ -3716,7 +3606,7 @@
       <c r="K29" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L29" s="63"/>
+      <c r="L29" s="39"/>
       <c r="M29" s="30"/>
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
@@ -3731,15 +3621,14 @@
       <c r="X29" s="30"/>
       <c r="Y29" s="30"/>
       <c r="Z29" s="30"/>
-      <c r="AA29" s="30"/>
-      <c r="AB29" s="30"/>
-      <c r="AC29" s="30"/>
-      <c r="AD29" s="18"/>
-    </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B30" s="29"/>
-      <c r="C30" s="23" t="s">
-        <v>235</v>
+      <c r="AA29" s="18"/>
+    </row>
+    <row r="30" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="23">
+        <v>1</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>245</v>
       </c>
       <c r="D30" s="34"/>
       <c r="E30" s="28"/>
@@ -3747,10 +3636,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="K30" s="23" t="s">
         <v>156</v>
-      </c>
-      <c r="K30" s="23" t="s">
-        <v>157</v>
       </c>
       <c r="L30" s="27"/>
       <c r="M30" s="30"/>
@@ -3767,15 +3656,14 @@
       <c r="X30" s="30"/>
       <c r="Y30" s="30"/>
       <c r="Z30" s="30"/>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="30"/>
-      <c r="AC30" s="30"/>
-      <c r="AD30" s="18"/>
-    </row>
-    <row r="31" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" s="23"/>
+      <c r="AA30" s="18"/>
+    </row>
+    <row r="31" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="23">
+        <v>2</v>
+      </c>
       <c r="C31" s="25" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="27"/>
@@ -3783,10 +3671,10 @@
         <v>2</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K31" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L31" s="27"/>
       <c r="M31" s="30"/>
@@ -3803,15 +3691,14 @@
       <c r="X31" s="30"/>
       <c r="Y31" s="30"/>
       <c r="Z31" s="30"/>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="30"/>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="18"/>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B32" s="23"/>
-      <c r="C32" s="23" t="s">
-        <v>237</v>
+      <c r="AA31" s="18"/>
+    </row>
+    <row r="32" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="23">
+        <v>3</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>248</v>
       </c>
       <c r="E32" s="27"/>
       <c r="K32" s="30"/>
@@ -3830,12 +3717,15 @@
       <c r="X32" s="30"/>
       <c r="Y32" s="30"/>
       <c r="Z32" s="30"/>
-      <c r="AA32" s="30"/>
-      <c r="AB32" s="30"/>
-      <c r="AC32" s="30"/>
-      <c r="AD32" s="18"/>
-    </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA32" s="18"/>
+    </row>
+    <row r="33" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="23">
+        <v>4</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>247</v>
+      </c>
       <c r="D33" s="28"/>
       <c r="E33" s="27"/>
       <c r="K33" s="30"/>
@@ -3854,23 +3744,22 @@
       <c r="X33" s="30"/>
       <c r="Y33" s="30"/>
       <c r="Z33" s="30"/>
-      <c r="AA33" s="30"/>
-      <c r="AB33" s="30"/>
-      <c r="AC33" s="30"/>
-      <c r="AD33" s="18"/>
-    </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B34" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="C34" s="50"/>
+      <c r="AA33" s="18"/>
+    </row>
+    <row r="34" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="23">
+        <v>5</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>249</v>
+      </c>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
-      <c r="I34" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
+      <c r="I34" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
       <c r="L34" s="28"/>
       <c r="M34" s="30"/>
       <c r="N34" s="30"/>
@@ -3886,17 +3775,14 @@
       <c r="X34" s="30"/>
       <c r="Y34" s="30"/>
       <c r="Z34" s="30"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="30"/>
-      <c r="AC34" s="30"/>
-      <c r="AD34" s="18"/>
-    </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B35" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>146</v>
+      <c r="AA34" s="18"/>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B35" s="23">
+        <v>6</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>250</v>
       </c>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
@@ -3909,7 +3795,7 @@
       <c r="K35" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L35" s="63"/>
+      <c r="L35" s="39"/>
       <c r="M35" s="30"/>
       <c r="N35" s="30"/>
       <c r="O35" s="30"/>
@@ -3924,25 +3810,24 @@
       <c r="X35" s="30"/>
       <c r="Y35" s="30"/>
       <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
-      <c r="AC35" s="30"/>
-      <c r="AD35" s="18"/>
-    </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B36" s="32"/>
-      <c r="C36" s="23" t="s">
-        <v>235</v>
+      <c r="AA35" s="18"/>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B36" s="23">
+        <v>7</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>251</v>
       </c>
       <c r="D36" s="27"/>
       <c r="I36" s="23">
         <v>1</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L36" s="27"/>
       <c r="M36" s="30"/>
@@ -3959,25 +3844,24 @@
       <c r="X36" s="30"/>
       <c r="Y36" s="30"/>
       <c r="Z36" s="30"/>
-      <c r="AA36" s="30"/>
-      <c r="AB36" s="30"/>
-      <c r="AC36" s="30"/>
-      <c r="AD36" s="18"/>
-    </row>
-    <row r="37" spans="2:30" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="23"/>
+      <c r="AA36" s="18"/>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B37" s="23">
+        <v>8</v>
+      </c>
       <c r="C37" s="25" t="s">
-        <v>236</v>
+        <v>140</v>
       </c>
       <c r="D37" s="27"/>
       <c r="I37" s="23">
         <v>2</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K37" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L37" s="27"/>
       <c r="M37" s="30"/>
@@ -3994,25 +3878,18 @@
       <c r="X37" s="30"/>
       <c r="Y37" s="30"/>
       <c r="Z37" s="30"/>
-      <c r="AA37" s="30"/>
-      <c r="AB37" s="30"/>
-      <c r="AC37" s="30"/>
-      <c r="AD37" s="18"/>
-    </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B38" s="23"/>
-      <c r="C38" s="23" t="s">
-        <v>237</v>
-      </c>
+      <c r="AA37" s="18"/>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D38" s="27"/>
       <c r="I38" s="23">
         <v>2</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L38" s="27"/>
       <c r="M38" s="30"/>
@@ -4029,12 +3906,13 @@
       <c r="X38" s="30"/>
       <c r="Y38" s="30"/>
       <c r="Z38" s="30"/>
-      <c r="AA38" s="30"/>
-      <c r="AB38" s="30"/>
-      <c r="AC38" s="30"/>
-      <c r="AD38" s="18"/>
-    </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="AA38" s="18"/>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B39" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="52"/>
       <c r="D39" s="27"/>
       <c r="M39" s="30"/>
       <c r="N39" s="30"/>
@@ -4050,16 +3928,15 @@
       <c r="X39" s="30"/>
       <c r="Y39" s="30"/>
       <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="30"/>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="18"/>
-    </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B40" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="C40" s="48"/>
+      <c r="AA39" s="18"/>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>146</v>
+      </c>
       <c r="D40" s="31"/>
       <c r="M40" s="30"/>
       <c r="N40" s="30"/>
@@ -4075,97 +3952,74 @@
       <c r="X40" s="30"/>
       <c r="Y40" s="30"/>
       <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="18"/>
-    </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B41" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>146</v>
+      <c r="AA40" s="18"/>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B41" s="29"/>
+      <c r="C41" s="23" t="s">
+        <v>233</v>
       </c>
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
       <c r="P41" s="30"/>
       <c r="Q41" s="30"/>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B42" s="23">
-        <v>1</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>133</v>
+    <row r="42" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="23"/>
+      <c r="C42" s="25" t="s">
+        <v>234</v>
       </c>
       <c r="D42" s="28"/>
       <c r="H42" s="28"/>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B43" s="23">
-        <v>2</v>
-      </c>
+    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B43" s="23"/>
       <c r="C43" s="23" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
       <c r="D43" s="27"/>
       <c r="H43" s="33"/>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B44" s="23">
-        <v>3</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>135</v>
-      </c>
+    <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D44" s="27"/>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B45" s="23">
-        <v>4</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>136</v>
-      </c>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B45" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="54"/>
       <c r="D45" s="27"/>
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B46" s="23">
-        <v>5</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>137</v>
+    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B46" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B47" s="23">
-        <v>6</v>
-      </c>
+    <row r="47" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B47" s="32"/>
       <c r="C47" s="23" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
       <c r="D47" s="28"/>
       <c r="H47" s="27"/>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B48" s="23">
-        <v>7</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>139</v>
+    <row r="48" spans="2:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="23"/>
+      <c r="C48" s="25" t="s">
+        <v>234</v>
       </c>
       <c r="D48" s="27"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="23">
-        <v>8</v>
-      </c>
+      <c r="B49" s="23"/>
       <c r="C49" s="23" t="s">
-        <v>140</v>
+        <v>235</v>
       </c>
       <c r="D49" s="27"/>
     </row>
@@ -4200,11 +4054,11 @@
       <c r="D60" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="S2:W2"/>
@@ -4212,7 +4066,6 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="I22:K22"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="I28:K28"/>

</xml_diff>

<commit_message>
Need fiend mistake into generic repository
</commit_message>
<xml_diff>
--- a/docs/Таблицы для БД.xlsx
+++ b/docs/Таблицы для БД.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\KPandDP\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43964C26-D433-440A-BBA6-CBEFBB038150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795C4EEA-343C-4BF8-89A0-3D4FDBE76F2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="253">
   <si>
     <t>Журнал ПОО</t>
   </si>
@@ -1042,13 +1042,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1066,6 +1066,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1074,9 +1077,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1428,14 +1428,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="E2" s="48" t="s">
+      <c r="C2" s="47"/>
+      <c r="E2" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="48"/>
+      <c r="F2" s="49"/>
       <c r="H2" s="45" t="s">
         <v>44</v>
       </c>
@@ -1744,30 +1744,30 @@
       <c r="F15" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="47"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="8"/>
       <c r="K15" s="50" t="s">
         <v>42</v>
       </c>
       <c r="L15" s="51"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="47" t="s">
+      <c r="N15" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="O15" s="47"/>
+      <c r="O15" s="48"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="47" t="s">
+      <c r="Q15" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="47"/>
+      <c r="R15" s="48"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="47" t="s">
+      <c r="T15" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="U15" s="47"/>
+      <c r="U15" s="48"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16" s="45" t="s">
@@ -1928,10 +1928,10 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="6"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12" t="s">
@@ -2521,10 +2521,10 @@
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="49"/>
+      <c r="C40" s="47"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
@@ -2569,10 +2569,10 @@
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="49" t="s">
+      <c r="B50" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="49"/>
+      <c r="C50" s="47"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
@@ -2624,6 +2624,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B10:C10"/>
@@ -2640,9 +2643,6 @@
     <mergeCell ref="Q15:R15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="H15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="285" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2653,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2693,16 +2693,16 @@
         <v>239</v>
       </c>
       <c r="C2" s="62"/>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="57"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="18"/>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="55" t="s">
         <v>244</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="40"/>
       <c r="N2" s="60" t="s">
         <v>147</v>
@@ -2710,17 +2710,18 @@
       <c r="O2" s="60"/>
       <c r="P2" s="60"/>
       <c r="Q2" s="38"/>
-      <c r="S2" s="55" t="s">
+      <c r="S2" s="56" t="s">
         <v>150</v>
       </c>
       <c r="T2" s="59"/>
       <c r="U2" s="59"/>
       <c r="V2" s="59"/>
-      <c r="W2" s="56"/>
-      <c r="Z2" s="55" t="s">
+      <c r="W2" s="59"/>
+      <c r="X2" s="57"/>
+      <c r="Z2" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="AA2" s="56"/>
+      <c r="AA2" s="57"/>
     </row>
     <row r="3" spans="2:27" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
@@ -2770,6 +2771,9 @@
       </c>
       <c r="W3" s="37" t="s">
         <v>205</v>
+      </c>
+      <c r="X3" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="Z3" s="19" t="s">
         <v>149</v>
@@ -2819,6 +2823,7 @@
       <c r="U4" s="23"/>
       <c r="V4" s="23"/>
       <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
       <c r="Z4" s="23">
         <v>1</v>
       </c>
@@ -2867,6 +2872,7 @@
       <c r="U5" s="23"/>
       <c r="V5" s="23"/>
       <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
       <c r="Z5" s="23">
         <v>2</v>
       </c>
@@ -2915,6 +2921,7 @@
       <c r="U6" s="23"/>
       <c r="V6" s="23"/>
       <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
       <c r="Z6" s="23">
         <v>3</v>
       </c>
@@ -2963,6 +2970,7 @@
       <c r="U7" s="23"/>
       <c r="V7" s="23"/>
       <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
       <c r="Z7" s="23">
         <v>4</v>
       </c>
@@ -3025,10 +3033,10 @@
       <c r="L9" s="44"/>
     </row>
     <row r="10" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="55" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="55"/>
       <c r="F10" s="24">
         <v>7</v>
       </c>
@@ -3191,6 +3199,12 @@
         <v>225</v>
       </c>
       <c r="D16" s="27"/>
+      <c r="F16" s="23">
+        <v>13</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>146</v>
+      </c>
       <c r="H16" s="18"/>
       <c r="I16" s="23">
         <v>13</v>
@@ -3561,10 +3575,10 @@
       <c r="AA27" s="18"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="55" t="s">
         <v>252</v>
       </c>
-      <c r="C28" s="58"/>
+      <c r="C28" s="55"/>
       <c r="D28" s="27"/>
       <c r="E28" s="31"/>
       <c r="I28" s="52" t="s">
@@ -4061,7 +4075,6 @@
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="S2:W2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
@@ -4069,6 +4082,7 @@
     <mergeCell ref="I22:K22"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="I28:K28"/>
+    <mergeCell ref="S2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="285" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>